<commit_message>
different shade names and gem table
Signed-off-by: Kori238 <jakeedwards238@gmail.com>
</commit_message>
<xml_diff>
--- a/GemCombinations.xlsx
+++ b/GemCombinations.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CrystalCaverns\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakee\Documents\CrystalCaverns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D0EECE-3502-445B-8110-0B0868A59371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6466BE-17BC-4643-84C0-CBFDC8EBC3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Family outlines" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Gem Families:</t>
   </si>
@@ -91,9 +91,6 @@
     <t>igniting and applying burning (whenever you ignite this deal damage equal to the stack, then reduce the stack by 1)</t>
   </si>
   <si>
-    <t>applying fortitude (target takes 25% less damage, reduce stack by 1 when target takes damage) weakness (target takes 25% more damage, reduce stack by 1 when target takes damage)</t>
-  </si>
-  <si>
     <t>applying armour/ energy cheat</t>
   </si>
   <si>
@@ -109,20 +106,38 @@
     <t>unique gem effects that do not belong to a family or should not be effected by family modifiers</t>
   </si>
   <si>
-    <t>bloodthirst bonuses and applying bleeding (if a target is bleeding, bloodthirst effects are active) (target takes damage equal to the stack at the end of turn (stack does not decrease naturally))</t>
-  </si>
-  <si>
-    <t>Necromancy? Souls? Summon allies????? - difficult to code? If I do code this do I want other gems to be able to summon things too?? Maybe allies can be a possibility too? Darkness?</t>
-  </si>
-  <si>
-    <t>a little Health restoration or ? Light?</t>
+    <t>applying fortitude (target takes 25% less damage, reduce stack by 1 when target takes damage) vulnerability (target takes 25% more damage, reduce stack by 1 when target takes damage)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> apply strength (target deals 25% more damage, reduce stack by 1 when target deals damage) apply weakness (target deals 25% less damage, reduce stack by 1 when target deals damage)</t>
+  </si>
+  <si>
+    <t>applies darkness (no effect) other black gems can use this resource by consuming it</t>
+  </si>
+  <si>
+    <t>applies blessings to self and has benificial effects based on blessings // number of blessings and a little health restoration</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Deal 4 damage</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,8 +145,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,8 +166,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA9EEC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -226,11 +278,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -258,6 +458,75 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -266,6 +535,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEA9EEC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -542,18 +816,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="53.140625" customWidth="1"/>
-    <col min="3" max="3" width="109.5703125" customWidth="1"/>
+    <col min="2" max="2" width="53.109375" customWidth="1"/>
+    <col min="3" max="3" width="109.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -569,15 +843,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -585,7 +859,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -593,7 +867,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -601,7 +875,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -609,7 +883,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -617,7 +891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -625,7 +899,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -633,7 +907,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -641,38 +915,387 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B53102D-E069-4539-BD35-AE73A5167F9A}">
+  <dimension ref="B1:Y14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="4" max="9" width="31.33203125" customWidth="1"/>
+    <col min="10" max="14" width="31.109375" customWidth="1"/>
+    <col min="15" max="23" width="30.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:25" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="17"/>
+    </row>
+    <row r="2" spans="2:25" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="24"/>
+    </row>
+    <row r="3" spans="2:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="24"/>
+    </row>
+    <row r="4" spans="2:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="24"/>
+    </row>
+    <row r="5" spans="2:25" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="24"/>
+    </row>
+    <row r="6" spans="2:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="24"/>
+    </row>
+    <row r="7" spans="2:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="24"/>
+    </row>
+    <row r="8" spans="2:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="24"/>
+    </row>
+    <row r="9" spans="2:25" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="24"/>
+    </row>
+    <row r="10" spans="2:25" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="23"/>
+      <c r="Y10" s="24"/>
+    </row>
+    <row r="11" spans="2:25" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="23"/>
+      <c r="Y11" s="24"/>
+    </row>
+    <row r="12" spans="2:25" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="29"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="31"/>
+    </row>
+    <row r="13" spans="2:25" ht="44.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
gem stuff Signed-off-by: Kori238 <jakeedwards238@gmail.com>
</commit_message>
<xml_diff>
--- a/GemCombinations.xlsx
+++ b/GemCombinations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CrystalCaverns\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakee\Documents\CrystalCaverns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F927C4E-9192-464A-AFD3-2212473CE83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C10D28-ADD9-417E-880A-A1B6E5223F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8520" yWindow="0" windowWidth="20385" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8916" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Family outlines" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
   <si>
     <t>Gem Families:</t>
   </si>
@@ -428,16 +428,110 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Silver</t>
+    <t>Keywords:</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <r>
+      <t>Pebble</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (2) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Draw 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Gray </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Draw</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Smoke </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Draw 2 then random discard 1.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Frost</t>
     </r>
     <r>
       <rPr>
@@ -457,6 +551,901 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Generate 2 White Gem. They cost 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Snow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Deal 3x [# cards played this turn] damage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lead </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Draw. Deal 2x [# of cards drawn this turn] damage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pewter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Draw. Gain 3x [# of cards drawn this turn] armour</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alabaster</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Deal 5 damage. This is 3x if you have played no other cards this turn</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Seashell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Gain 8 armour. This is 3x if you have played no other cards this turn</t>
+    </r>
+  </si>
+  <si>
+    <t>Persistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You do not discard this at the end of your turn </t>
+  </si>
+  <si>
+    <t>Twin</t>
+  </si>
+  <si>
+    <t>Generate a free copy of this card without this keyword</t>
+  </si>
+  <si>
+    <t>Generate a free copy of this card without this keyword at the start of your next turn</t>
+  </si>
+  <si>
+    <t>Recurring</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Champagne</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Gain 8 armour. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Twin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Porcelain </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Deal 5 damage. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Twin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ivory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(X)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Deal 10 damage to random targets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> times, occasionally yourself! </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Persistant</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Beige</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(-)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This is a copy of the last card you played -- cannot be merged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pearl </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Gain 5x [# cards played this turn] armour</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Magnolia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Deal 3 damage then gain 5 armour</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Eggshell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Deal 4 damage.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Cleave</t>
+    </r>
+  </si>
+  <si>
+    <t>Cleave</t>
+  </si>
+  <si>
+    <t>Effects all enemies</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Spring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Gain 8 armour. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recurring</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Coconut</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Deal 5 damage. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recurring</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chiffon</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(X)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Deal 2x </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">X </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">damage. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cleave</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Peppermint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Deal 3 damage gain 4 armour </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cleave</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Merino </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Gain 4 armour </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cleave</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Scorpion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Draw a card </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cleave</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Marengo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>(0)</t>
     </r>
     <r>
@@ -467,50 +1456,156 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> Draw a card. Gain 1 energy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nevada</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(0) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Draw cards until your hand is full, after you play your next card discard your hand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Silver </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> Gain 1 energy</t>
     </r>
   </si>
   <si>
-    <t>Keywords:</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <r>
-      <t>Pebble</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (2) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Draw 2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Gray </t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Porpoise</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Your next card costs 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Shadow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -530,51 +1625,31 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Draw</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Smoke </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(1) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Draw 2 then random discard 1.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Frost</t>
+      <t xml:space="preserve"> Draw a card for each card you've played this turn </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Persistant</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nickel</t>
     </r>
     <r>
       <rPr>
@@ -599,44 +1674,99 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Generate 2 White Gem. They cost 0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Pearl </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(2) Gain 5x [# cards played this turn] armour</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Snow</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Draw a card. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recurring</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Arsenic </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Double your energy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Ash </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(2) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Draw 4 random discard 2 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Anchor</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -651,42 +1781,69 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(2)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Deal 3x [# cards played this turn] damage</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Lead </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(2)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Draw. Deal 2x [# of cards drawn this turn] damage</t>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Discard your hand then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Draw 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fog</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (X) Draw X cards and give them </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Temporary Persistent</t>
     </r>
   </si>
 </sst>
@@ -694,7 +1851,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -731,6 +1888,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
       <name val="Calibri"/>
@@ -777,12 +1942,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -922,21 +2087,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1071,7 +2221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1110,19 +2260,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1137,68 +2275,98 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1488,18 +2656,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="53.140625" customWidth="1"/>
-    <col min="3" max="3" width="109.5703125" customWidth="1"/>
+    <col min="2" max="2" width="53.109375" customWidth="1"/>
+    <col min="3" max="3" width="109.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1507,7 +2675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1515,7 +2683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1523,7 +2691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1531,7 +2699,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1539,7 +2707,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1547,7 +2715,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1555,7 +2723,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1563,7 +2731,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1571,7 +2739,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1579,7 +2747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1587,7 +2755,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1595,7 +2763,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1603,7 +2771,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1611,7 +2779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="10" t="s">
         <v>24</v>
       </c>
@@ -1619,82 +2787,98 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="44" t="s">
+    <row r="17" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="45" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="42"/>
-      <c r="C19" s="43"/>
-    </row>
-    <row r="20" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-    </row>
-    <row r="21" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
-    </row>
-    <row r="22" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="38"/>
-      <c r="C22" s="39"/>
-    </row>
-    <row r="23" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
-    </row>
-    <row r="24" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="38"/>
-      <c r="C24" s="39"/>
-    </row>
-    <row r="25" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="38"/>
-      <c r="C25" s="39"/>
-    </row>
-    <row r="26" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="38"/>
-      <c r="C26" s="39"/>
-    </row>
-    <row r="27" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
-    </row>
-    <row r="28" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="38"/>
-      <c r="C28" s="39"/>
-    </row>
-    <row r="29" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
-    </row>
-    <row r="30" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
-    </row>
-    <row r="31" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="38"/>
-      <c r="C31" s="39"/>
-    </row>
-    <row r="32" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="38"/>
-      <c r="C32" s="39"/>
-    </row>
-    <row r="33" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="38"/>
-      <c r="C33" s="39"/>
-    </row>
-    <row r="34" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="38"/>
-      <c r="C34" s="39"/>
-    </row>
-    <row r="35" spans="2:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="40"/>
-      <c r="C35" s="41"/>
+    </row>
+    <row r="19" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+    </row>
+    <row r="24" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+    </row>
+    <row r="25" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="42"/>
+      <c r="C25" s="43"/>
+    </row>
+    <row r="26" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="42"/>
+      <c r="C26" s="43"/>
+    </row>
+    <row r="27" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="42"/>
+      <c r="C27" s="43"/>
+    </row>
+    <row r="28" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="42"/>
+      <c r="C28" s="43"/>
+    </row>
+    <row r="29" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="42"/>
+      <c r="C29" s="43"/>
+    </row>
+    <row r="30" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="42"/>
+      <c r="C30" s="43"/>
+    </row>
+    <row r="31" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="42"/>
+      <c r="C31" s="43"/>
+    </row>
+    <row r="32" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="42"/>
+      <c r="C32" s="43"/>
+    </row>
+    <row r="33" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="42"/>
+      <c r="C33" s="43"/>
+    </row>
+    <row r="34" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="42"/>
+      <c r="C34" s="43"/>
+    </row>
+    <row r="35" spans="2:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="44"/>
+      <c r="C35" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1705,23 +2889,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B53102D-E069-4539-BD35-AE73A5167F9A}">
   <dimension ref="B1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="4" max="9" width="31.28515625" customWidth="1"/>
-    <col min="10" max="14" width="31.140625" customWidth="1"/>
-    <col min="15" max="23" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="4" max="9" width="31.33203125" customWidth="1"/>
+    <col min="10" max="14" width="31.109375" customWidth="1"/>
+    <col min="15" max="25" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:25" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="24" t="s">
         <v>30</v>
       </c>
       <c r="E1" s="12" t="s">
@@ -1733,346 +2917,394 @@
       <c r="G1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="35" t="s">
+      <c r="H1" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1" s="47" t="s">
+      <c r="L1" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="17"/>
-    </row>
-    <row r="2" spans="2:25" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P1" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="T1" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="X1" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y1" s="38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="2:25" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="24"/>
-    </row>
-    <row r="3" spans="2:25" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="R2" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="S2" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="U2" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="V2" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="X2" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y2" s="47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="22"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="24"/>
-    </row>
-    <row r="4" spans="2:25" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="36"/>
+      <c r="Y3" s="36"/>
+    </row>
+    <row r="4" spans="2:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="24"/>
-    </row>
-    <row r="5" spans="2:25" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+    </row>
+    <row r="5" spans="2:25" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="22"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="22"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="24"/>
-    </row>
-    <row r="6" spans="2:25" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="36"/>
+      <c r="Y5" s="36"/>
+    </row>
+    <row r="6" spans="2:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="22"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="24"/>
-    </row>
-    <row r="7" spans="2:25" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="36"/>
+      <c r="Y6" s="36"/>
+    </row>
+    <row r="7" spans="2:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="24"/>
-    </row>
-    <row r="8" spans="2:25" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="36"/>
+      <c r="Y7" s="36"/>
+    </row>
+    <row r="8" spans="2:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="22"/>
-      <c r="U8" s="22"/>
-      <c r="V8" s="22"/>
-      <c r="W8" s="22"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="24"/>
-    </row>
-    <row r="9" spans="2:25" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="36"/>
+      <c r="Y8" s="36"/>
+    </row>
+    <row r="9" spans="2:25" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="22"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
-      <c r="W9" s="22"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="24"/>
-    </row>
-    <row r="10" spans="2:25" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="36"/>
+      <c r="Y9" s="36"/>
+    </row>
+    <row r="10" spans="2:25" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="22"/>
-      <c r="V10" s="22"/>
-      <c r="W10" s="22"/>
-      <c r="X10" s="23"/>
-      <c r="Y10" s="24"/>
-    </row>
-    <row r="11" spans="2:25" ht="44.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="36"/>
+      <c r="Y10" s="36"/>
+    </row>
+    <row r="11" spans="2:25" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="22"/>
-      <c r="U11" s="22"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="22"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="24"/>
-    </row>
-    <row r="12" spans="2:25" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="36"/>
+      <c r="Y11" s="36"/>
+    </row>
+    <row r="12" spans="2:25" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="30"/>
-      <c r="Y12" s="31"/>
-    </row>
-    <row r="13" spans="2:25" ht="44.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:25" ht="43.15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="37"/>
+      <c r="Y12" s="37"/>
+    </row>
+    <row r="13" spans="2:25" ht="44.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
basic isometric grid and character setup
Signed-off-by: Jake <jakeedwards238@gmail.com>
</commit_message>
<xml_diff>
--- a/GemCombinations.xlsx
+++ b/GemCombinations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CrystalCaverns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CD5D26-FB32-4828-8C82-D4BF6C6D80F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2899B1CB-7926-47EC-93C3-C87F1652C4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9135" yWindow="0" windowWidth="19770" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Family outlines" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
   <si>
     <t>Gem Families:</t>
   </si>
@@ -1372,6 +1372,562 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Marengo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Draw a card. Gain 1 energy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nevada</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(0) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Draw cards until your hand is full, after you play your next card discard your hand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Silver </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Gain 1 energy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Porpoise</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Your next card costs 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Shadow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Draw a card for each card you've played this turn </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Persistant</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nickel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Draw a card. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recurring</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Arsenic </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Double your energy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Ash </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(2) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Draw 4 random discard 2 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Anchor</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Discard your hand then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Draw 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fog</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (X) Draw X cards and give them </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Temporary Persistent</t>
+    </r>
+  </si>
+  <si>
+    <t>Temporary &lt;keyword&gt;</t>
+  </si>
+  <si>
+    <t>Loses the specified keyword after use</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Flint </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(2) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Draw </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cleave</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Dove </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(2) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Draw 2 cards and give them </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Temporary Persistent</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Chrome </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(0)  Gain 1 energy at the start of your next turn </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recurring</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Scorpion</t>
     </r>
     <r>
@@ -1413,508 +1969,49 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Persistant. Twin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Platinum </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(1)  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Gain 1 energy </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Cleave</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Marengo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(0)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Draw a card. Gain 1 energy</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nevada</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(0) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Draw cards until your hand is full, after you play your next card discard your hand</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Silver </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(0)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Gain 1 energy</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Porpoise</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(1) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Your next card costs 0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Shadow</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(1)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Draw a card for each card you've played this turn </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Persistant</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nickel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(1)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Draw a card. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Recurring</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Arsenic </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(1)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Double your energy</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Ash </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(2) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Draw 4 random discard 2 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Anchor</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(1)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Discard your hand then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Draw 3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Fog</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (X) Draw X cards and give them </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Temporary Persistent</t>
-    </r>
-  </si>
-  <si>
-    <t>Temporary &lt;keyword&gt;</t>
-  </si>
-  <si>
-    <t>Loses the specified keyword after use</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Flint </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(2) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Draw </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cleave</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Dove </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(1) </t>
     </r>
   </si>
 </sst>
@@ -2727,7 +2824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B15" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
@@ -2901,10 +2998,10 @@
     </row>
     <row r="23" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="43" t="s">
         <v>79</v>
-      </c>
-      <c r="C23" s="43" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2964,8 +3061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B53102D-E069-4539-BD35-AE73A5167F9A}">
   <dimension ref="B1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3063,9 +3160,13 @@
       <c r="G2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="15"/>
+      <c r="H2" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="I2" s="15"/>
-      <c r="J2" s="16"/>
+      <c r="J2" s="34" t="s">
+        <v>82</v>
+      </c>
       <c r="K2" s="31" t="s">
         <v>44</v>
       </c>
@@ -3073,43 +3174,43 @@
         <v>45</v>
       </c>
       <c r="M2" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="N2" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="O2" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q2" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="S2" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="T2" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="V2" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="W2" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="R2" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="S2" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="T2" s="18" t="s">
+      <c r="X2" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="U2" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="V2" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="W2" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="X2" s="47" t="s">
+      <c r="Y2" s="47" t="s">
         <v>69</v>
-      </c>
-      <c r="Y2" s="47" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="2:25" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>